<commit_message>
Fix up students example
</commit_message>
<xml_diff>
--- a/data/students.xlsx
+++ b/data/students.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mine/Desktop/RStudio/r4ds/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20474076-2CEB-DC48-85B0-B29D061430E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A2C184-384A-D645-9987-A3B3BF34FF48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39620" yWindow="1940" windowWidth="21760" windowHeight="11440" xr2:uid="{A4001EB2-6D7D-9B4C-B59B-6DA6116F86C6}"/>
+    <workbookView xWindow="7040" yWindow="1940" windowWidth="21760" windowHeight="11440" xr2:uid="{A4001EB2-6D7D-9B4C-B59B-6DA6116F86C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Student ID</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>AGE</t>
-  </si>
-  <si>
-    <t>five</t>
   </si>
   <si>
     <t>N/A</t>
@@ -447,7 +444,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51724306-14EF-0442-BCA4-E04159FA09CB}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -517,7 +516,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -531,7 +530,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -553,8 +552,8 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
-        <v>15</v>
+      <c r="E6">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -562,10 +561,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Revert back to old dataset to match spreadsheets chapter
</commit_message>
<xml_diff>
--- a/data/students.xlsx
+++ b/data/students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mine/Desktop/RStudio/r4ds/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A2C184-384A-D645-9987-A3B3BF34FF48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D66A757-4349-FF4A-B677-2F5F1C0D3BFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7040" yWindow="1940" windowWidth="21760" windowHeight="11440" xr2:uid="{A4001EB2-6D7D-9B4C-B59B-6DA6116F86C6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Student ID</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Leon Rossini</t>
+  </si>
+  <si>
+    <t>five</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -552,8 +555,8 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="E6">
-        <v>5</v>
+      <c r="E6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>